<commit_message>
Add the rest of the test cases
</commit_message>
<xml_diff>
--- a/QA-testCases/MazeHaze_testCases.xlsx
+++ b/QA-testCases/MazeHaze_testCases.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Калина Нончева\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Калина Нончева\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DC2D3F4-2A98-436B-85DB-048D96F61219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FDB0D5-93BB-4E38-A302-26A3B54E6A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="8964" xr2:uid="{4D482C56-9218-4E5B-9115-E5B0D0D38CE7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{4D482C56-9218-4E5B-9115-E5B0D0D38CE7}"/>
   </bookViews>
   <sheets>
-    <sheet name="mazes.cpp" sheetId="2" r:id="rId1"/>
-    <sheet name="menu.cpp" sheetId="1" r:id="rId2"/>
+    <sheet name="menu.cpp" sheetId="2" r:id="rId1"/>
+    <sheet name="mazes.cpp" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="61">
   <si>
     <t>Tests - mazes.cpp</t>
   </si>
@@ -131,6 +131,93 @@
   </si>
   <si>
     <t>Shows the menu choices</t>
+  </si>
+  <si>
+    <t>Tests - menu.cpp</t>
+  </si>
+  <si>
+    <t>Test_05</t>
+  </si>
+  <si>
+    <t>clearLevel()</t>
+  </si>
+  <si>
+    <t>Desplays text when you rech 'X'</t>
+  </si>
+  <si>
+    <t>Test_06</t>
+  </si>
+  <si>
+    <t>playerAction()</t>
+  </si>
+  <si>
+    <t>Creates the player's movement</t>
+  </si>
+  <si>
+    <t>Starts the game</t>
+  </si>
+  <si>
+    <t>Entering key 'up'</t>
+  </si>
+  <si>
+    <t>Entering key 'down'</t>
+  </si>
+  <si>
+    <t>Entering key 'right'</t>
+  </si>
+  <si>
+    <t>Entering key 'left'</t>
+  </si>
+  <si>
+    <t>key 'up'</t>
+  </si>
+  <si>
+    <t>key 'down'</t>
+  </si>
+  <si>
+    <t>key 'right'</t>
+  </si>
+  <si>
+    <t>key 'left'</t>
+  </si>
+  <si>
+    <t>Moves up</t>
+  </si>
+  <si>
+    <t>Moves down</t>
+  </si>
+  <si>
+    <t>Moves right</t>
+  </si>
+  <si>
+    <t>Moves left</t>
+  </si>
+  <si>
+    <t>Test_07</t>
+  </si>
+  <si>
+    <t>mazeEasy()</t>
+  </si>
+  <si>
+    <t>Display difficulty level "Easy"</t>
+  </si>
+  <si>
+    <t>Test_08</t>
+  </si>
+  <si>
+    <t>mazeMedium()</t>
+  </si>
+  <si>
+    <t>Display difficulty level "Medium"</t>
+  </si>
+  <si>
+    <t>Test_09</t>
+  </si>
+  <si>
+    <t>mazeHard()</t>
+  </si>
+  <si>
+    <t>Display difficulty level "Hard"</t>
   </si>
 </sst>
 </file>
@@ -321,9 +408,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -335,46 +442,30 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="99">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -883,55 +974,81 @@
           <bgColor theme="9" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -942,55 +1059,81 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1030,6 +1173,841 @@
           <bgColor theme="9" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -1057,60 +2035,135 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F58A4F37-1EEA-4F1B-90C4-BBC235CF15F4}" name="Table612" displayName="Table612" ref="B10:G11" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" headerRowBorderDxfId="40" tableBorderDxfId="41" totalsRowBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F58A4F37-1EEA-4F1B-90C4-BBC235CF15F4}" name="Table612" displayName="Table612" ref="B10:G11" totalsRowShown="0" headerRowDxfId="98" dataDxfId="96" headerRowBorderDxfId="97" tableBorderDxfId="95" totalsRowBorderDxfId="94">
   <autoFilter ref="B10:G11" xr:uid="{F58A4F37-1EEA-4F1B-90C4-BBC235CF15F4}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F8CFF553-D617-433A-887D-D4743BDB5F82}" name="Number step" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{3B218E14-59F6-4699-90F5-7A6C3AB2C180}" name="Description" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{8D139E49-BB77-4FEB-9B72-45188CC039ED}" name="Test Data" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{5BC77B32-720C-436E-8DBD-B1BEF1FB57C9}" name="Expectations" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{2694AEB3-1DCD-489F-86A4-78D6F5B1F749}" name="Actual Result" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{A27E9FF8-9AF9-452C-AFF4-01B2DE40EF7A}" name="Status" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{F8CFF553-D617-433A-887D-D4743BDB5F82}" name="Number step" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{3B218E14-59F6-4699-90F5-7A6C3AB2C180}" name="Description" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{8D139E49-BB77-4FEB-9B72-45188CC039ED}" name="Test Data" dataDxfId="91"/>
+    <tableColumn id="4" xr3:uid="{5BC77B32-720C-436E-8DBD-B1BEF1FB57C9}" name="Expectations" dataDxfId="90"/>
+    <tableColumn id="5" xr3:uid="{2694AEB3-1DCD-489F-86A4-78D6F5B1F749}" name="Actual Result" dataDxfId="89"/>
+    <tableColumn id="6" xr3:uid="{A27E9FF8-9AF9-452C-AFF4-01B2DE40EF7A}" name="Status" dataDxfId="88"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4E6ABE80-395D-445C-A2C0-717BAC0537CF}" name="Table6123" displayName="Table6123" ref="B20:G21" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" headerRowBorderDxfId="29" tableBorderDxfId="30" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4E6ABE80-395D-445C-A2C0-717BAC0537CF}" name="Table6123" displayName="Table6123" ref="B20:G21" totalsRowShown="0" headerRowDxfId="87" dataDxfId="85" headerRowBorderDxfId="86" tableBorderDxfId="84" totalsRowBorderDxfId="83">
   <autoFilter ref="B20:G21" xr:uid="{4E6ABE80-395D-445C-A2C0-717BAC0537CF}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{449B4652-9758-4CFE-A8A5-60F3EFC8159D}" name="Number step" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{922F05C0-9AE8-4C4A-90B8-2866ACD9455D}" name="Description" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{2914BAB3-ED4D-4F32-B531-E32610ACD4BA}" name="Test Data" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{B4131B10-73E0-4FF6-BEC4-178EB1FC2926}" name="Expectations" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{0BE9F2CA-B342-4DC0-A327-C949F71F3596}" name="Actual Result" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{EE3532DA-0F8D-4B88-9834-8BBDED89AC40}" name="Status" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{449B4652-9758-4CFE-A8A5-60F3EFC8159D}" name="Number step" dataDxfId="82"/>
+    <tableColumn id="2" xr3:uid="{922F05C0-9AE8-4C4A-90B8-2866ACD9455D}" name="Description" dataDxfId="81"/>
+    <tableColumn id="3" xr3:uid="{2914BAB3-ED4D-4F32-B531-E32610ACD4BA}" name="Test Data" dataDxfId="80"/>
+    <tableColumn id="4" xr3:uid="{B4131B10-73E0-4FF6-BEC4-178EB1FC2926}" name="Expectations" dataDxfId="79"/>
+    <tableColumn id="5" xr3:uid="{0BE9F2CA-B342-4DC0-A327-C949F71F3596}" name="Actual Result" dataDxfId="78"/>
+    <tableColumn id="6" xr3:uid="{EE3532DA-0F8D-4B88-9834-8BBDED89AC40}" name="Status" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DF839241-D2B2-4A78-99BC-5E2BEEE1DEA1}" name="Table61234" displayName="Table61234" ref="B30:G31" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowBorderDxfId="18" tableBorderDxfId="19" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DF839241-D2B2-4A78-99BC-5E2BEEE1DEA1}" name="Table61234" displayName="Table61234" ref="B30:G31" totalsRowShown="0" headerRowDxfId="76" dataDxfId="74" headerRowBorderDxfId="75" tableBorderDxfId="73" totalsRowBorderDxfId="72">
   <autoFilter ref="B30:G31" xr:uid="{DF839241-D2B2-4A78-99BC-5E2BEEE1DEA1}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{34DFF587-CDE2-4688-A169-48C5D45D3FE1}" name="Number step" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{20127EC5-9103-4DAF-9F8D-8C20BBE1F165}" name="Description" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{EC5A676E-01C8-43BF-B51B-665D082AC738}" name="Test Data" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{55C52187-292D-4F2F-BB6C-AC4D719B7147}" name="Expectations" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{0E3D247B-BAC7-489F-BBBD-E2D4FD03E862}" name="Actual Result" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{E86D8427-E99A-4FFA-93B4-2717545985DE}" name="Status" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{34DFF587-CDE2-4688-A169-48C5D45D3FE1}" name="Number step" dataDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{20127EC5-9103-4DAF-9F8D-8C20BBE1F165}" name="Description" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{EC5A676E-01C8-43BF-B51B-665D082AC738}" name="Test Data" dataDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{55C52187-292D-4F2F-BB6C-AC4D719B7147}" name="Expectations" dataDxfId="68"/>
+    <tableColumn id="5" xr3:uid="{0E3D247B-BAC7-489F-BBBD-E2D4FD03E862}" name="Actual Result" dataDxfId="67"/>
+    <tableColumn id="6" xr3:uid="{E86D8427-E99A-4FFA-93B4-2717545985DE}" name="Status" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6AD289C8-3324-4C16-B67E-EF2E8853FC8F}" name="Table612345" displayName="Table612345" ref="B40:G41" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6AD289C8-3324-4C16-B67E-EF2E8853FC8F}" name="Table612345" displayName="Table612345" ref="B40:G41" totalsRowShown="0" headerRowDxfId="65" dataDxfId="63" headerRowBorderDxfId="64" tableBorderDxfId="62" totalsRowBorderDxfId="61">
   <autoFilter ref="B40:G41" xr:uid="{6AD289C8-3324-4C16-B67E-EF2E8853FC8F}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{CBFE011C-A219-401A-A28B-8BBBDA2B12A8}" name="Number step" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{E4EDAF63-3D32-4AA4-AC05-0294249CF7D1}" name="Description" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{29EE8141-2B9D-4C88-ACC5-69B0F0F63DCC}" name="Test Data" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{3F65A08B-4C04-4188-9011-ACBC1389877A}" name="Expectations" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{DF2F5940-59EE-474E-B7CA-671B043C1CAA}" name="Actual Result" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{E5AB8FDB-366E-40EB-9B35-E72A20D4B546}" name="Status" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{CBFE011C-A219-401A-A28B-8BBBDA2B12A8}" name="Number step" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{E4EDAF63-3D32-4AA4-AC05-0294249CF7D1}" name="Description" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{29EE8141-2B9D-4C88-ACC5-69B0F0F63DCC}" name="Test Data" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{3F65A08B-4C04-4188-9011-ACBC1389877A}" name="Expectations" dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{DF2F5940-59EE-474E-B7CA-671B043C1CAA}" name="Actual Result" dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{E5AB8FDB-366E-40EB-9B35-E72A20D4B546}" name="Status" dataDxfId="55"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{07ED605F-E422-445A-8979-A276C23461DA}" name="Table61236" displayName="Table61236" ref="B10:G11" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53" headerRowBorderDxfId="51" tableBorderDxfId="52" totalsRowBorderDxfId="50">
+  <autoFilter ref="B10:G11" xr:uid="{07ED605F-E422-445A-8979-A276C23461DA}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{FE2E35DA-0466-40E0-9558-A35E613195CD}" name="Number step" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{DEA3120C-50E6-490E-88E7-DC711E76DB10}" name="Description" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{68322B8C-94F6-487F-A8E9-F505C3570926}" name="Test Data" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{94FB3D41-9585-4CAA-9EFD-7B16485383BD}" name="Expectations" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{CF55C739-CA07-4B88-92E5-141FC258FAE6}" name="Actual Result" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{06972DA9-C68E-40A4-A56F-4B99C5C31B6D}" name="Status" dataDxfId="44"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{447F7C98-4666-4D7F-8EFC-D9E7439BAABC}" name="Table612367" displayName="Table612367" ref="B20:G25" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" headerRowBorderDxfId="40" tableBorderDxfId="41" totalsRowBorderDxfId="39">
+  <autoFilter ref="B20:G25" xr:uid="{447F7C98-4666-4D7F-8EFC-D9E7439BAABC}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{BC437E72-61B3-4408-A220-01F24B47C009}" name="Number step" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{A1702984-48A9-44F2-8BA1-A518F8AF586E}" name="Description" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{710FEA1C-45DF-4355-88AC-CF5DD04F696A}" name="Test Data" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{52ED93EA-2DAB-4DEC-88F6-B1347C8A0255}" name="Expectations" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{BA7AA056-E63A-45FD-81EE-BD476318E130}" name="Actual Result" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{09F0746E-4C31-467B-AD1C-B02D5855F5CC}" name="Status" dataDxfId="33"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A75E37EC-E1E3-44DB-8A42-DF830CA6787C}" name="Table612368" displayName="Table612368" ref="B34:G35" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" headerRowBorderDxfId="29" tableBorderDxfId="30" totalsRowBorderDxfId="28">
+  <autoFilter ref="B34:G35" xr:uid="{A75E37EC-E1E3-44DB-8A42-DF830CA6787C}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{6FAC3D8A-9D98-4F04-B597-5033C2C7F886}" name="Number step" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{CCD75399-88B4-4095-A7EF-56E1E6084C21}" name="Description" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{55A1FAFC-350B-4AD9-B38E-D90F099D5B9E}" name="Test Data" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{252D05CA-D9A6-46CF-B58B-8FC5AB113BB6}" name="Expectations" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{C3006CE0-6E10-4717-AA39-61F5504F4C6F}" name="Actual Result" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{64D6F26D-C845-4FAE-89BE-A76C8D34EA00}" name="Status" dataDxfId="22"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{C02EC1FE-00D3-4D8A-AAB7-5DA85F1B6136}" name="Table6123689" displayName="Table6123689" ref="B44:G45" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" headerRowBorderDxfId="18" tableBorderDxfId="19" totalsRowBorderDxfId="17">
+  <autoFilter ref="B44:G45" xr:uid="{C02EC1FE-00D3-4D8A-AAB7-5DA85F1B6136}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{903DD499-1F5D-4150-8462-5F037F102938}" name="Number step" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{6B9202F9-3A6B-4F07-834F-BCB6EDD68B6E}" name="Description" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{AFFF592A-942B-40F0-9C8C-2458EE7F1EC5}" name="Test Data" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{4F40742C-66B8-4418-8863-98C461FEC18C}" name="Expectations" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{BD9F6E10-707F-4A18-984F-6E42EAC50A14}" name="Actual Result" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{D415E9A7-B315-4F0C-85D7-8042544C1851}" name="Status" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{FB672CF3-E2AB-4783-AFE1-102C89738D21}" name="Table612368910" displayName="Table612368910" ref="B54:G55" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+  <autoFilter ref="B54:G55" xr:uid="{FB672CF3-E2AB-4783-AFE1-102C89738D21}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{AD479A22-31AE-4CE7-AE12-8717BEC36EAF}" name="Number step" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{D24E54AB-BD2F-4C14-9125-C90B1A5FD442}" name="Description" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{AAD5C521-ECCF-4957-9C46-519F03DA0482}" name="Test Data" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{D67289C3-BB52-4128-B195-17D74CDF7A60}" name="Expectations" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{08D9310B-F98A-46F1-B6DA-0D99642E0EB0}" name="Actual Result" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{663D5941-D21F-4F82-8D42-72197981AA67}" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1415,8 +2468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF6B5021-6499-437D-9356-1F5412B4C41D}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1430,462 +2483,462 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
+      <c r="A1" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="21"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="3">
         <v>44388.622916666667</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="5" t="s">
+      <c r="B7" s="18"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="3">
         <v>44388.625</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="14"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="18">
+      <c r="B11" s="7">
         <v>1</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="19" t="s">
+      <c r="D11" s="9"/>
+      <c r="E11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="3">
         <v>44388.625694444447</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="5" t="s">
+      <c r="B17" s="18"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="3">
         <v>44388.633333333331</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="14"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="18">
+      <c r="B21" s="7">
         <v>1</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="19" t="s">
+      <c r="D21" s="9"/>
+      <c r="E21" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="19" t="s">
+      <c r="F21" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="21" t="s">
+      <c r="G21" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="4"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="16"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="3">
         <v>44388.634027777778</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="9"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="5" t="s">
+      <c r="B27" s="18"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="3">
         <v>44388.636805555558</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="14"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="F30" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G30" s="17" t="s">
+      <c r="G30" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="18">
+      <c r="B31" s="7">
         <v>1</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="20"/>
-      <c r="E31" s="19" t="s">
+      <c r="D31" s="9"/>
+      <c r="E31" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F31" s="19" t="s">
+      <c r="F31" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G31" s="21" t="s">
+      <c r="G31" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="4"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="16"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="11">
+      <c r="E35" s="3">
         <v>44388.637499999997</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="9"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="5" t="s">
+      <c r="B37" s="18"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="11">
+      <c r="E37" s="3">
         <v>44388.64166666667</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="14"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="13"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="16" t="s">
+      <c r="C40" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="D40" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E40" s="16" t="s">
+      <c r="E40" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F40" s="16" t="s">
+      <c r="F40" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G40" s="17" t="s">
+      <c r="G40" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B41" s="18">
+      <c r="B41" s="7">
         <v>1</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="20"/>
-      <c r="E41" s="19" t="s">
+      <c r="D41" s="9"/>
+      <c r="E41" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F41" s="19" t="s">
+      <c r="F41" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G41" s="21" t="s">
+      <c r="G41" s="10" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B9:G9"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="C26:C27"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="B39:G39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="4">
@@ -1899,14 +2952,678 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4771A7A8-873D-4BAE-9C7F-D11600FFC469}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3">
+        <v>44388.666666666664</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="18"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3">
+        <v>44388.670138888891</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="7">
+        <v>1</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="3">
+        <v>44388.67083333333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="18"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="3">
+        <v>44388.677777777775</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="13"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="22">
+        <v>1</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="23"/>
+      <c r="E21" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="8">
+        <v>2</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="8">
+        <v>3</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="8">
+        <v>4</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="8">
+        <v>5</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="16"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="3">
+        <v>44388.677777777775</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="18"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="3">
+        <v>44388.681250000001</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="13"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="7">
+        <v>1</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="9"/>
+      <c r="E35" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B37" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="16"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="3">
+        <v>44388.681944444441</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B40" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B41" s="18"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="3">
+        <v>44388.68472222222</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B43" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="13"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B44" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B45" s="7">
+        <v>1</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="9"/>
+      <c r="E45" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B47" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="16"/>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B49" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="3">
+        <v>44388.682638888888</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B50" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B51" s="18"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="3">
+        <v>44388.686111111114</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B53" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="13"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B54" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B55" s="7">
+        <v>1</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D55" s="9"/>
+      <c r="E55" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B13:E13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="5">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>